<commit_message>
Update DU for 27 SEP
</commit_message>
<xml_diff>
--- a/testing/Test Cases.xlsx
+++ b/testing/Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="8265" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="153">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -630,9 +630,6 @@
     <t>Biding (add)</t>
   </si>
   <si>
-    <t>Validate that student can add a bid successfully by keying in a correct course code and section in round 1</t>
-  </si>
-  <si>
     <t>Validate that in round1 , student cannot bid a module which is not offered by his own school</t>
   </si>
   <si>
@@ -686,6 +683,24 @@
   </si>
   <si>
     <t>Login Failed with error meassage displayed "Incorrect userid or password!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that student cannot add a module which class timelot for that section clash with that of a previous bidded section </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that student cannot add a module which exam timelot for that section clash with that of a previous bidded section </t>
+  </si>
+  <si>
+    <t>Validate that stduent cannot add a module as he has not compeleted the prerequisite for that module</t>
+  </si>
+  <si>
+    <t>Validate that student cannot add a module which he has completed</t>
+  </si>
+  <si>
+    <t>Bidding(add - round 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that student cannot add a module </t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1067,7 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10351,8 +10366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10427,7 +10442,7 @@
         <v>89</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>91</v>
@@ -10436,10 +10451,10 @@
         <v>92</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10453,7 +10468,7 @@
         <v>103</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>91</v>
@@ -10462,10 +10477,10 @@
         <v>97</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -10488,10 +10503,10 @@
         <v>98</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10505,7 +10520,7 @@
         <v>114</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>91</v>
@@ -10514,10 +10529,10 @@
         <v>97</v>
       </c>
       <c r="G5" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10531,7 +10546,7 @@
         <v>115</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>91</v>
@@ -10540,10 +10555,10 @@
         <v>98</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10557,7 +10572,7 @@
         <v>100</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>91</v>
@@ -10566,10 +10581,10 @@
         <v>101</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10583,7 +10598,7 @@
         <v>95</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>91</v>
@@ -10592,10 +10607,10 @@
         <v>102</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10618,10 +10633,10 @@
         <v>104</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10644,10 +10659,10 @@
         <v>105</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="51" x14ac:dyDescent="0.2">
@@ -10661,7 +10676,7 @@
         <v>110</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>91</v>
@@ -10670,10 +10685,10 @@
         <v>112</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="63.75" x14ac:dyDescent="0.2">
@@ -10687,7 +10702,7 @@
         <v>111</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>91</v>
@@ -10696,10 +10711,10 @@
         <v>113</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -10713,7 +10728,7 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10861,10 +10876,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10929,7 +10944,7 @@
         <v>128</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="38.25" x14ac:dyDescent="0.2">
@@ -10937,7 +10952,7 @@
         <v>128</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="38.25" x14ac:dyDescent="0.2">
@@ -10945,31 +10960,31 @@
         <v>128</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>128</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>128</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="38.25" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>128</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="38.25" x14ac:dyDescent="0.2">
@@ -10977,7 +10992,46 @@
         <v>128</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>